<commit_message>
Export leaderboards as Excel
</commit_message>
<xml_diff>
--- a/backend/participants.xlsx
+++ b/backend/participants.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="16">
   <si>
     <t>Rank</t>
   </si>
@@ -25,28 +25,37 @@
     <t>Developer</t>
   </si>
   <si>
+    <t>Ensan 3ayesh mn zaman</t>
+  </si>
+  <si>
+    <t>moo moo</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Lolo Amr</t>
+  </si>
+  <si>
+    <t>Alaa Amr</t>
+  </si>
+  <si>
+    <t>Habiba Gamil</t>
+  </si>
+  <si>
+    <t>Mariam Wael</t>
+  </si>
+  <si>
+    <t>Salma Abosabie</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Britney Spears</t>
+  </si>
+  <si>
     <t>Mohamed Ahmed</t>
-  </si>
-  <si>
-    <t>Habiba Gamil</t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>Alaa Amr</t>
-  </si>
-  <si>
-    <t>Mariam Wael</t>
-  </si>
-  <si>
-    <t>Salma Abosabie</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>Britney Spears</t>
   </si>
   <si>
     <t>Michael jackson</t>
@@ -426,7 +435,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D14"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="3" width="30" customWidth="1"/>
@@ -452,7 +461,10 @@
         <v>4</v>
       </c>
       <c r="C2">
-        <v>50</v>
+        <v>620</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -463,7 +475,7 @@
         <v>5</v>
       </c>
       <c r="C3">
-        <v>50</v>
+        <v>150</v>
       </c>
       <c r="D3" t="s">
         <v>6</v>
@@ -477,7 +489,7 @@
         <v>7</v>
       </c>
       <c r="C4">
-        <v>50</v>
+        <v>110</v>
       </c>
       <c r="D4" t="s">
         <v>6</v>
@@ -505,10 +517,10 @@
         <v>9</v>
       </c>
       <c r="C6">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="D6" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -516,13 +528,13 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C7">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="D7" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -530,13 +542,13 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8" t="s">
         <v>12</v>
-      </c>
-      <c r="C8">
-        <v>50</v>
-      </c>
-      <c r="D8" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -544,13 +556,13 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="C9">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="D9" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -558,10 +570,10 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="C10">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="D10" t="s">
         <v>6</v>
@@ -572,13 +584,13 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="C11">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D11" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -586,13 +598,10 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>4</v>
-      </c>
-      <c r="C12">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D12" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -600,13 +609,21 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>4</v>
-      </c>
-      <c r="C13">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D13" t="s">
-        <v>6</v>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>